<commit_message>
100ppi spot number upgrade to 45, and modified accordingly.
</commit_message>
<xml_diff>
--- a/database/SpotData.xlsx
+++ b/database/SpotData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="163">
   <si>
     <t>日期</t>
   </si>
@@ -423,6 +423,87 @@
   <si>
     <t>20180213</t>
   </si>
+  <si>
+    <t>20180222</t>
+  </si>
+  <si>
+    <t>20180223</t>
+  </si>
+  <si>
+    <t>20180226</t>
+  </si>
+  <si>
+    <t>20180227</t>
+  </si>
+  <si>
+    <t>20180228</t>
+  </si>
+  <si>
+    <t>20180301</t>
+  </si>
+  <si>
+    <t>20180302</t>
+  </si>
+  <si>
+    <t>20180305</t>
+  </si>
+  <si>
+    <t>20180306</t>
+  </si>
+  <si>
+    <t>20180307</t>
+  </si>
+  <si>
+    <t>20180308</t>
+  </si>
+  <si>
+    <t>20180309</t>
+  </si>
+  <si>
+    <t>20180312</t>
+  </si>
+  <si>
+    <t>20180313</t>
+  </si>
+  <si>
+    <t>20180314</t>
+  </si>
+  <si>
+    <t>20180315</t>
+  </si>
+  <si>
+    <t>20180316</t>
+  </si>
+  <si>
+    <t>20180319</t>
+  </si>
+  <si>
+    <t>20180320</t>
+  </si>
+  <si>
+    <t>20180321</t>
+  </si>
+  <si>
+    <t>20180322</t>
+  </si>
+  <si>
+    <t>20180323</t>
+  </si>
+  <si>
+    <t>20180326</t>
+  </si>
+  <si>
+    <t>20180327</t>
+  </si>
+  <si>
+    <t>20180328</t>
+  </si>
+  <si>
+    <t>20180329</t>
+  </si>
+  <si>
+    <t>20180330</t>
+  </si>
 </sst>
 </file>
 
@@ -779,7 +860,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AT92"/>
+  <dimension ref="A1:AT119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -13662,6 +13743,3786 @@
         <v>2417.27</v>
       </c>
     </row>
+    <row r="93" spans="1:46">
+      <c r="A93" s="1">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>136</v>
+      </c>
+      <c r="C93">
+        <v>52290</v>
+      </c>
+      <c r="D93">
+        <v>3924</v>
+      </c>
+      <c r="E93">
+        <v>26600</v>
+      </c>
+      <c r="F93">
+        <v>13715</v>
+      </c>
+      <c r="G93">
+        <v>271.39</v>
+      </c>
+      <c r="H93">
+        <v>4231.11</v>
+      </c>
+      <c r="I93">
+        <v>3963.33</v>
+      </c>
+      <c r="J93">
+        <v>11745.5</v>
+      </c>
+      <c r="K93">
+        <v>19250</v>
+      </c>
+      <c r="L93">
+        <v>3620</v>
+      </c>
+      <c r="M93">
+        <v>2843.33</v>
+      </c>
+      <c r="N93">
+        <v>4117.69</v>
+      </c>
+      <c r="O93">
+        <v>102150</v>
+      </c>
+      <c r="P93">
+        <v>148000</v>
+      </c>
+      <c r="Q93">
+        <v>5714.55</v>
+      </c>
+      <c r="R93">
+        <v>6258</v>
+      </c>
+      <c r="S93">
+        <v>15663.7</v>
+      </c>
+      <c r="T93">
+        <v>2528</v>
+      </c>
+      <c r="U93">
+        <v>6518.33</v>
+      </c>
+      <c r="V93">
+        <v>2616.67</v>
+      </c>
+      <c r="W93">
+        <v>1543.2</v>
+      </c>
+      <c r="X93">
+        <v>2355</v>
+      </c>
+      <c r="Y93">
+        <v>5490</v>
+      </c>
+      <c r="Z93">
+        <v>3000</v>
+      </c>
+      <c r="AA93">
+        <v>2709</v>
+      </c>
+      <c r="AB93">
+        <v>7204.55</v>
+      </c>
+      <c r="AC93">
+        <v>8131.25</v>
+      </c>
+      <c r="AD93">
+        <v>2855</v>
+      </c>
+      <c r="AE93">
+        <v>740.8</v>
+      </c>
+      <c r="AF93">
+        <v>5160</v>
+      </c>
+      <c r="AG93">
+        <v>6450</v>
+      </c>
+      <c r="AH93">
+        <v>9655</v>
+      </c>
+      <c r="AI93">
+        <v>3660</v>
+      </c>
+      <c r="AJ93">
+        <v>3068.57</v>
+      </c>
+      <c r="AK93">
+        <v>5637.5</v>
+      </c>
+      <c r="AL93">
+        <v>1781.07</v>
+      </c>
+      <c r="AM93">
+        <v>1880</v>
+      </c>
+      <c r="AN93">
+        <v>1498.33</v>
+      </c>
+      <c r="AO93">
+        <v>548.67</v>
+      </c>
+      <c r="AP93">
+        <v>4230</v>
+      </c>
+      <c r="AQ93">
+        <v>122.67</v>
+      </c>
+      <c r="AR93">
+        <v>75</v>
+      </c>
+      <c r="AS93">
+        <v>9183.33</v>
+      </c>
+      <c r="AT93">
+        <v>2418.18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:46">
+      <c r="A94" s="1">
+        <v>92</v>
+      </c>
+      <c r="B94" t="s">
+        <v>137</v>
+      </c>
+      <c r="C94">
+        <v>53070</v>
+      </c>
+      <c r="D94">
+        <v>3920</v>
+      </c>
+      <c r="E94">
+        <v>26930</v>
+      </c>
+      <c r="F94">
+        <v>13970</v>
+      </c>
+      <c r="G94">
+        <v>272.2</v>
+      </c>
+      <c r="H94">
+        <v>4232.22</v>
+      </c>
+      <c r="I94">
+        <v>3941.67</v>
+      </c>
+      <c r="J94">
+        <v>11772.7</v>
+      </c>
+      <c r="K94">
+        <v>19400</v>
+      </c>
+      <c r="L94">
+        <v>3622.67</v>
+      </c>
+      <c r="M94">
+        <v>2846.67</v>
+      </c>
+      <c r="N94">
+        <v>4100</v>
+      </c>
+      <c r="O94">
+        <v>104150</v>
+      </c>
+      <c r="P94">
+        <v>147250</v>
+      </c>
+      <c r="Q94">
+        <v>5884.55</v>
+      </c>
+      <c r="R94">
+        <v>6258</v>
+      </c>
+      <c r="S94">
+        <v>15664</v>
+      </c>
+      <c r="T94">
+        <v>2528</v>
+      </c>
+      <c r="U94">
+        <v>6525</v>
+      </c>
+      <c r="V94">
+        <v>2616.67</v>
+      </c>
+      <c r="W94">
+        <v>1544.8</v>
+      </c>
+      <c r="X94">
+        <v>2363.33</v>
+      </c>
+      <c r="Y94">
+        <v>5490</v>
+      </c>
+      <c r="Z94">
+        <v>3000</v>
+      </c>
+      <c r="AA94">
+        <v>2709</v>
+      </c>
+      <c r="AB94">
+        <v>7177.27</v>
+      </c>
+      <c r="AC94">
+        <v>8131.25</v>
+      </c>
+      <c r="AD94">
+        <v>2880</v>
+      </c>
+      <c r="AE94">
+        <v>734.4</v>
+      </c>
+      <c r="AF94">
+        <v>5160</v>
+      </c>
+      <c r="AG94">
+        <v>6450</v>
+      </c>
+      <c r="AH94">
+        <v>9605</v>
+      </c>
+      <c r="AI94">
+        <v>3660</v>
+      </c>
+      <c r="AJ94">
+        <v>3064.29</v>
+      </c>
+      <c r="AK94">
+        <v>5682.5</v>
+      </c>
+      <c r="AL94">
+        <v>1781.79</v>
+      </c>
+      <c r="AM94">
+        <v>1880</v>
+      </c>
+      <c r="AN94">
+        <v>1498.33</v>
+      </c>
+      <c r="AO94">
+        <v>550.5599999999999</v>
+      </c>
+      <c r="AP94">
+        <v>4175</v>
+      </c>
+      <c r="AQ94">
+        <v>122.67</v>
+      </c>
+      <c r="AR94">
+        <v>75</v>
+      </c>
+      <c r="AS94">
+        <v>9150</v>
+      </c>
+      <c r="AT94">
+        <v>2418.18</v>
+      </c>
+    </row>
+    <row r="95" spans="1:46">
+      <c r="A95" s="1">
+        <v>93</v>
+      </c>
+      <c r="B95" t="s">
+        <v>138</v>
+      </c>
+      <c r="C95">
+        <v>52950</v>
+      </c>
+      <c r="D95">
+        <v>4042.14</v>
+      </c>
+      <c r="E95">
+        <v>26930</v>
+      </c>
+      <c r="F95">
+        <v>13910</v>
+      </c>
+      <c r="G95">
+        <v>272.95</v>
+      </c>
+      <c r="H95">
+        <v>4348.89</v>
+      </c>
+      <c r="I95">
+        <v>3988.33</v>
+      </c>
+      <c r="J95">
+        <v>12031.8</v>
+      </c>
+      <c r="K95">
+        <v>19400</v>
+      </c>
+      <c r="L95">
+        <v>3632.5</v>
+      </c>
+      <c r="M95">
+        <v>2846.67</v>
+      </c>
+      <c r="N95">
+        <v>4194.17</v>
+      </c>
+      <c r="O95">
+        <v>103650</v>
+      </c>
+      <c r="P95">
+        <v>146750</v>
+      </c>
+      <c r="Q95">
+        <v>5990.91</v>
+      </c>
+      <c r="R95">
+        <v>6218</v>
+      </c>
+      <c r="S95">
+        <v>15651.6</v>
+      </c>
+      <c r="T95">
+        <v>2520</v>
+      </c>
+      <c r="U95">
+        <v>6538.33</v>
+      </c>
+      <c r="V95">
+        <v>2616.67</v>
+      </c>
+      <c r="W95">
+        <v>1548</v>
+      </c>
+      <c r="X95">
+        <v>2403.33</v>
+      </c>
+      <c r="Y95">
+        <v>5490</v>
+      </c>
+      <c r="Z95">
+        <v>3000</v>
+      </c>
+      <c r="AA95">
+        <v>2709</v>
+      </c>
+      <c r="AB95">
+        <v>7045</v>
+      </c>
+      <c r="AC95">
+        <v>8143.75</v>
+      </c>
+      <c r="AD95">
+        <v>2837.5</v>
+      </c>
+      <c r="AE95">
+        <v>728.8</v>
+      </c>
+      <c r="AF95">
+        <v>5215</v>
+      </c>
+      <c r="AG95">
+        <v>6450</v>
+      </c>
+      <c r="AH95">
+        <v>9565</v>
+      </c>
+      <c r="AI95">
+        <v>3660</v>
+      </c>
+      <c r="AJ95">
+        <v>3081.43</v>
+      </c>
+      <c r="AK95">
+        <v>5736.25</v>
+      </c>
+      <c r="AL95">
+        <v>1787.14</v>
+      </c>
+      <c r="AM95">
+        <v>1960</v>
+      </c>
+      <c r="AN95">
+        <v>1498.33</v>
+      </c>
+      <c r="AO95">
+        <v>561.33</v>
+      </c>
+      <c r="AP95">
+        <v>4090</v>
+      </c>
+      <c r="AQ95">
+        <v>122.67</v>
+      </c>
+      <c r="AR95">
+        <v>75</v>
+      </c>
+      <c r="AS95">
+        <v>9062.5</v>
+      </c>
+      <c r="AT95">
+        <v>2420.91</v>
+      </c>
+    </row>
+    <row r="96" spans="1:46">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="B96" t="s">
+        <v>139</v>
+      </c>
+      <c r="C96">
+        <v>52920</v>
+      </c>
+      <c r="D96">
+        <v>4055.71</v>
+      </c>
+      <c r="E96">
+        <v>27000</v>
+      </c>
+      <c r="F96">
+        <v>13950</v>
+      </c>
+      <c r="G96">
+        <v>272</v>
+      </c>
+      <c r="H96">
+        <v>4366.67</v>
+      </c>
+      <c r="I96">
+        <v>3988.33</v>
+      </c>
+      <c r="J96">
+        <v>12163.6</v>
+      </c>
+      <c r="K96">
+        <v>19550</v>
+      </c>
+      <c r="L96">
+        <v>3652</v>
+      </c>
+      <c r="M96">
+        <v>2846.67</v>
+      </c>
+      <c r="N96">
+        <v>4195.83</v>
+      </c>
+      <c r="O96">
+        <v>104450</v>
+      </c>
+      <c r="P96">
+        <v>147000</v>
+      </c>
+      <c r="Q96">
+        <v>6015.45</v>
+      </c>
+      <c r="R96">
+        <v>6178</v>
+      </c>
+      <c r="S96">
+        <v>15647.3</v>
+      </c>
+      <c r="T96">
+        <v>2502</v>
+      </c>
+      <c r="U96">
+        <v>6515</v>
+      </c>
+      <c r="V96">
+        <v>2616.67</v>
+      </c>
+      <c r="W96">
+        <v>1548</v>
+      </c>
+      <c r="X96">
+        <v>2411.67</v>
+      </c>
+      <c r="Y96">
+        <v>5490</v>
+      </c>
+      <c r="Z96">
+        <v>3000</v>
+      </c>
+      <c r="AA96">
+        <v>2709</v>
+      </c>
+      <c r="AB96">
+        <v>7045</v>
+      </c>
+      <c r="AC96">
+        <v>8156.25</v>
+      </c>
+      <c r="AD96">
+        <v>2727.5</v>
+      </c>
+      <c r="AE96">
+        <v>724</v>
+      </c>
+      <c r="AF96">
+        <v>5265</v>
+      </c>
+      <c r="AG96">
+        <v>6450</v>
+      </c>
+      <c r="AH96">
+        <v>9565</v>
+      </c>
+      <c r="AI96">
+        <v>3652</v>
+      </c>
+      <c r="AJ96">
+        <v>3077.14</v>
+      </c>
+      <c r="AK96">
+        <v>5730</v>
+      </c>
+      <c r="AL96">
+        <v>1790.71</v>
+      </c>
+      <c r="AM96">
+        <v>1960</v>
+      </c>
+      <c r="AN96">
+        <v>1498.33</v>
+      </c>
+      <c r="AO96">
+        <v>566.4400000000001</v>
+      </c>
+      <c r="AP96">
+        <v>4050</v>
+      </c>
+      <c r="AQ96">
+        <v>122.67</v>
+      </c>
+      <c r="AR96">
+        <v>75</v>
+      </c>
+      <c r="AS96">
+        <v>9062.5</v>
+      </c>
+      <c r="AT96">
+        <v>2420.91</v>
+      </c>
+    </row>
+    <row r="97" spans="1:46">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="B97" t="s">
+        <v>140</v>
+      </c>
+      <c r="C97">
+        <v>52430</v>
+      </c>
+      <c r="D97">
+        <v>4059.29</v>
+      </c>
+      <c r="E97">
+        <v>26700</v>
+      </c>
+      <c r="F97">
+        <v>14045</v>
+      </c>
+      <c r="G97">
+        <v>270.01</v>
+      </c>
+      <c r="H97">
+        <v>4367.78</v>
+      </c>
+      <c r="I97">
+        <v>3988.33</v>
+      </c>
+      <c r="J97">
+        <v>12163.6</v>
+      </c>
+      <c r="K97">
+        <v>19300</v>
+      </c>
+      <c r="L97">
+        <v>3611</v>
+      </c>
+      <c r="M97">
+        <v>2846.67</v>
+      </c>
+      <c r="N97">
+        <v>4185</v>
+      </c>
+      <c r="O97">
+        <v>104250</v>
+      </c>
+      <c r="P97">
+        <v>147250</v>
+      </c>
+      <c r="Q97">
+        <v>5995.45</v>
+      </c>
+      <c r="R97">
+        <v>6154</v>
+      </c>
+      <c r="S97">
+        <v>15647.7</v>
+      </c>
+      <c r="T97">
+        <v>2496</v>
+      </c>
+      <c r="U97">
+        <v>6506.67</v>
+      </c>
+      <c r="V97">
+        <v>2616.67</v>
+      </c>
+      <c r="W97">
+        <v>1548</v>
+      </c>
+      <c r="X97">
+        <v>2421.67</v>
+      </c>
+      <c r="Y97">
+        <v>5490</v>
+      </c>
+      <c r="Z97">
+        <v>3000</v>
+      </c>
+      <c r="AA97">
+        <v>2709</v>
+      </c>
+      <c r="AB97">
+        <v>6860</v>
+      </c>
+      <c r="AC97">
+        <v>8256.25</v>
+      </c>
+      <c r="AD97">
+        <v>2640</v>
+      </c>
+      <c r="AE97">
+        <v>712.8</v>
+      </c>
+      <c r="AF97">
+        <v>5267.5</v>
+      </c>
+      <c r="AG97">
+        <v>6450</v>
+      </c>
+      <c r="AH97">
+        <v>9555</v>
+      </c>
+      <c r="AI97">
+        <v>3652</v>
+      </c>
+      <c r="AJ97">
+        <v>3111.43</v>
+      </c>
+      <c r="AK97">
+        <v>5722.5</v>
+      </c>
+      <c r="AL97">
+        <v>1793.21</v>
+      </c>
+      <c r="AM97">
+        <v>1976.67</v>
+      </c>
+      <c r="AN97">
+        <v>1498.33</v>
+      </c>
+      <c r="AO97">
+        <v>564</v>
+      </c>
+      <c r="AP97">
+        <v>3950</v>
+      </c>
+      <c r="AQ97">
+        <v>122.67</v>
+      </c>
+      <c r="AR97">
+        <v>75</v>
+      </c>
+      <c r="AS97">
+        <v>9058.33</v>
+      </c>
+      <c r="AT97">
+        <v>2425.45</v>
+      </c>
+    </row>
+    <row r="98" spans="1:46">
+      <c r="A98" s="1">
+        <v>96</v>
+      </c>
+      <c r="B98" t="s">
+        <v>141</v>
+      </c>
+      <c r="C98">
+        <v>52050</v>
+      </c>
+      <c r="D98">
+        <v>4088.12</v>
+      </c>
+      <c r="E98">
+        <v>26730</v>
+      </c>
+      <c r="F98">
+        <v>14140</v>
+      </c>
+      <c r="G98">
+        <v>270.09</v>
+      </c>
+      <c r="H98">
+        <v>4402.5</v>
+      </c>
+      <c r="I98">
+        <v>3988.33</v>
+      </c>
+      <c r="J98">
+        <v>12118.2</v>
+      </c>
+      <c r="K98">
+        <v>19200</v>
+      </c>
+      <c r="L98">
+        <v>3609</v>
+      </c>
+      <c r="M98">
+        <v>2853.33</v>
+      </c>
+      <c r="N98">
+        <v>4190.83</v>
+      </c>
+      <c r="O98">
+        <v>103550</v>
+      </c>
+      <c r="P98">
+        <v>146750</v>
+      </c>
+      <c r="Q98">
+        <v>5995.45</v>
+      </c>
+      <c r="R98">
+        <v>6124</v>
+      </c>
+      <c r="S98">
+        <v>15655.6</v>
+      </c>
+      <c r="T98">
+        <v>2496</v>
+      </c>
+      <c r="U98">
+        <v>6510</v>
+      </c>
+      <c r="V98">
+        <v>2616.67</v>
+      </c>
+      <c r="W98">
+        <v>1548</v>
+      </c>
+      <c r="X98">
+        <v>2421.67</v>
+      </c>
+      <c r="Y98">
+        <v>5490</v>
+      </c>
+      <c r="Z98">
+        <v>3000</v>
+      </c>
+      <c r="AA98">
+        <v>2709</v>
+      </c>
+      <c r="AB98">
+        <v>6789.09</v>
+      </c>
+      <c r="AC98">
+        <v>8371.43</v>
+      </c>
+      <c r="AD98">
+        <v>2600</v>
+      </c>
+      <c r="AE98">
+        <v>706.4</v>
+      </c>
+      <c r="AF98">
+        <v>5297.5</v>
+      </c>
+      <c r="AG98">
+        <v>6450</v>
+      </c>
+      <c r="AH98">
+        <v>9565</v>
+      </c>
+      <c r="AI98">
+        <v>3652</v>
+      </c>
+      <c r="AJ98">
+        <v>3147.14</v>
+      </c>
+      <c r="AK98">
+        <v>5731.25</v>
+      </c>
+      <c r="AL98">
+        <v>1798.57</v>
+      </c>
+      <c r="AM98">
+        <v>1976.67</v>
+      </c>
+      <c r="AN98">
+        <v>1498.33</v>
+      </c>
+      <c r="AO98">
+        <v>561</v>
+      </c>
+      <c r="AP98">
+        <v>3890</v>
+      </c>
+      <c r="AQ98">
+        <v>122.67</v>
+      </c>
+      <c r="AR98">
+        <v>75</v>
+      </c>
+      <c r="AS98">
+        <v>9041.67</v>
+      </c>
+      <c r="AT98">
+        <v>2426.36</v>
+      </c>
+    </row>
+    <row r="99" spans="1:46">
+      <c r="A99" s="1">
+        <v>97</v>
+      </c>
+      <c r="B99" t="s">
+        <v>142</v>
+      </c>
+      <c r="C99">
+        <v>51960</v>
+      </c>
+      <c r="D99">
+        <v>4085.62</v>
+      </c>
+      <c r="E99">
+        <v>26490</v>
+      </c>
+      <c r="F99">
+        <v>14140</v>
+      </c>
+      <c r="G99">
+        <v>270.9</v>
+      </c>
+      <c r="H99">
+        <v>4393.75</v>
+      </c>
+      <c r="I99">
+        <v>3980</v>
+      </c>
+      <c r="J99">
+        <v>12140.9</v>
+      </c>
+      <c r="K99">
+        <v>19000</v>
+      </c>
+      <c r="L99">
+        <v>3613</v>
+      </c>
+      <c r="M99">
+        <v>2853.33</v>
+      </c>
+      <c r="N99">
+        <v>4179.17</v>
+      </c>
+      <c r="O99">
+        <v>101800</v>
+      </c>
+      <c r="P99">
+        <v>146500</v>
+      </c>
+      <c r="Q99">
+        <v>6038.18</v>
+      </c>
+      <c r="R99">
+        <v>6104</v>
+      </c>
+      <c r="S99">
+        <v>15657</v>
+      </c>
+      <c r="T99">
+        <v>2496</v>
+      </c>
+      <c r="U99">
+        <v>6541.67</v>
+      </c>
+      <c r="V99">
+        <v>2616.67</v>
+      </c>
+      <c r="W99">
+        <v>1549.6</v>
+      </c>
+      <c r="X99">
+        <v>2515</v>
+      </c>
+      <c r="Y99">
+        <v>5490</v>
+      </c>
+      <c r="Z99">
+        <v>3000</v>
+      </c>
+      <c r="AA99">
+        <v>2709</v>
+      </c>
+      <c r="AB99">
+        <v>6789.09</v>
+      </c>
+      <c r="AC99">
+        <v>8371.43</v>
+      </c>
+      <c r="AD99">
+        <v>2555</v>
+      </c>
+      <c r="AE99">
+        <v>697.6</v>
+      </c>
+      <c r="AF99">
+        <v>5300</v>
+      </c>
+      <c r="AG99">
+        <v>6479.17</v>
+      </c>
+      <c r="AH99">
+        <v>9565</v>
+      </c>
+      <c r="AI99">
+        <v>3652</v>
+      </c>
+      <c r="AJ99">
+        <v>3217.14</v>
+      </c>
+      <c r="AK99">
+        <v>5803.75</v>
+      </c>
+      <c r="AL99">
+        <v>1806.79</v>
+      </c>
+      <c r="AM99">
+        <v>1976.67</v>
+      </c>
+      <c r="AN99">
+        <v>1498.33</v>
+      </c>
+      <c r="AO99">
+        <v>562.11</v>
+      </c>
+      <c r="AP99">
+        <v>3830</v>
+      </c>
+      <c r="AQ99">
+        <v>121</v>
+      </c>
+      <c r="AR99">
+        <v>74.83</v>
+      </c>
+      <c r="AS99">
+        <v>9054.17</v>
+      </c>
+      <c r="AT99">
+        <v>2429.09</v>
+      </c>
+    </row>
+    <row r="100" spans="1:46">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="B100" t="s">
+        <v>143</v>
+      </c>
+      <c r="C100">
+        <v>51770</v>
+      </c>
+      <c r="D100">
+        <v>4044</v>
+      </c>
+      <c r="E100">
+        <v>26330</v>
+      </c>
+      <c r="F100">
+        <v>14000</v>
+      </c>
+      <c r="G100">
+        <v>271.6</v>
+      </c>
+      <c r="H100">
+        <v>4366.25</v>
+      </c>
+      <c r="I100">
+        <v>3980</v>
+      </c>
+      <c r="J100">
+        <v>12168.2</v>
+      </c>
+      <c r="K100">
+        <v>18900</v>
+      </c>
+      <c r="L100">
+        <v>3639.67</v>
+      </c>
+      <c r="M100">
+        <v>2856.67</v>
+      </c>
+      <c r="N100">
+        <v>4161.67</v>
+      </c>
+      <c r="O100">
+        <v>101800</v>
+      </c>
+      <c r="P100">
+        <v>146500</v>
+      </c>
+      <c r="Q100">
+        <v>6035.45</v>
+      </c>
+      <c r="R100">
+        <v>6102</v>
+      </c>
+      <c r="S100">
+        <v>15658.4</v>
+      </c>
+      <c r="T100">
+        <v>2496</v>
+      </c>
+      <c r="U100">
+        <v>6541.67</v>
+      </c>
+      <c r="V100">
+        <v>2616.67</v>
+      </c>
+      <c r="W100">
+        <v>1549.6</v>
+      </c>
+      <c r="X100">
+        <v>2506.67</v>
+      </c>
+      <c r="Y100">
+        <v>5490</v>
+      </c>
+      <c r="Z100">
+        <v>3000</v>
+      </c>
+      <c r="AA100">
+        <v>2709</v>
+      </c>
+      <c r="AB100">
+        <v>6689.09</v>
+      </c>
+      <c r="AC100">
+        <v>8371.43</v>
+      </c>
+      <c r="AD100">
+        <v>2555</v>
+      </c>
+      <c r="AE100">
+        <v>695.8</v>
+      </c>
+      <c r="AF100">
+        <v>5282.5</v>
+      </c>
+      <c r="AG100">
+        <v>6479.17</v>
+      </c>
+      <c r="AH100">
+        <v>9565</v>
+      </c>
+      <c r="AI100">
+        <v>3652</v>
+      </c>
+      <c r="AJ100">
+        <v>3224.29</v>
+      </c>
+      <c r="AK100">
+        <v>5822.5</v>
+      </c>
+      <c r="AL100">
+        <v>1815.71</v>
+      </c>
+      <c r="AM100">
+        <v>1976.67</v>
+      </c>
+      <c r="AN100">
+        <v>1498.33</v>
+      </c>
+      <c r="AO100">
+        <v>557.4400000000001</v>
+      </c>
+      <c r="AP100">
+        <v>3760</v>
+      </c>
+      <c r="AQ100">
+        <v>121</v>
+      </c>
+      <c r="AR100">
+        <v>74.83</v>
+      </c>
+      <c r="AS100">
+        <v>9054.17</v>
+      </c>
+      <c r="AT100">
+        <v>2430.91</v>
+      </c>
+    </row>
+    <row r="101" spans="1:46">
+      <c r="A101" s="1">
+        <v>99</v>
+      </c>
+      <c r="B101" t="s">
+        <v>144</v>
+      </c>
+      <c r="C101">
+        <v>51860</v>
+      </c>
+      <c r="D101">
+        <v>4011.33</v>
+      </c>
+      <c r="E101">
+        <v>25780</v>
+      </c>
+      <c r="F101">
+        <v>14080</v>
+      </c>
+      <c r="G101">
+        <v>271.45</v>
+      </c>
+      <c r="H101">
+        <v>4321.25</v>
+      </c>
+      <c r="I101">
+        <v>3980</v>
+      </c>
+      <c r="J101">
+        <v>12181.8</v>
+      </c>
+      <c r="K101">
+        <v>18650</v>
+      </c>
+      <c r="L101">
+        <v>3623.67</v>
+      </c>
+      <c r="M101">
+        <v>2856.67</v>
+      </c>
+      <c r="N101">
+        <v>4152.5</v>
+      </c>
+      <c r="O101">
+        <v>101900</v>
+      </c>
+      <c r="P101">
+        <v>146000</v>
+      </c>
+      <c r="Q101">
+        <v>6041.82</v>
+      </c>
+      <c r="R101">
+        <v>6102</v>
+      </c>
+      <c r="S101">
+        <v>15658.4</v>
+      </c>
+      <c r="T101">
+        <v>2522</v>
+      </c>
+      <c r="U101">
+        <v>6538.33</v>
+      </c>
+      <c r="V101">
+        <v>2616.67</v>
+      </c>
+      <c r="W101">
+        <v>1549.6</v>
+      </c>
+      <c r="X101">
+        <v>2523.33</v>
+      </c>
+      <c r="Y101">
+        <v>5490</v>
+      </c>
+      <c r="Z101">
+        <v>3000</v>
+      </c>
+      <c r="AA101">
+        <v>2709</v>
+      </c>
+      <c r="AB101">
+        <v>6689.09</v>
+      </c>
+      <c r="AC101">
+        <v>8371.43</v>
+      </c>
+      <c r="AD101">
+        <v>2550</v>
+      </c>
+      <c r="AE101">
+        <v>691</v>
+      </c>
+      <c r="AF101">
+        <v>5260</v>
+      </c>
+      <c r="AG101">
+        <v>6479.17</v>
+      </c>
+      <c r="AH101">
+        <v>9565</v>
+      </c>
+      <c r="AI101">
+        <v>3652</v>
+      </c>
+      <c r="AJ101">
+        <v>3235.71</v>
+      </c>
+      <c r="AK101">
+        <v>5820</v>
+      </c>
+      <c r="AL101">
+        <v>1829.29</v>
+      </c>
+      <c r="AM101">
+        <v>1976.67</v>
+      </c>
+      <c r="AN101">
+        <v>1498.33</v>
+      </c>
+      <c r="AO101">
+        <v>548</v>
+      </c>
+      <c r="AP101">
+        <v>3705</v>
+      </c>
+      <c r="AQ101">
+        <v>121.33</v>
+      </c>
+      <c r="AR101">
+        <v>74.67</v>
+      </c>
+      <c r="AS101">
+        <v>9054.17</v>
+      </c>
+      <c r="AT101">
+        <v>2438.18</v>
+      </c>
+    </row>
+    <row r="102" spans="1:46">
+      <c r="A102" s="1">
+        <v>100</v>
+      </c>
+      <c r="B102" t="s">
+        <v>145</v>
+      </c>
+      <c r="C102">
+        <v>51960</v>
+      </c>
+      <c r="D102">
+        <v>4004.29</v>
+      </c>
+      <c r="E102">
+        <v>25920</v>
+      </c>
+      <c r="F102">
+        <v>14080</v>
+      </c>
+      <c r="G102">
+        <v>272.86</v>
+      </c>
+      <c r="H102">
+        <v>4313.75</v>
+      </c>
+      <c r="I102">
+        <v>3980</v>
+      </c>
+      <c r="J102">
+        <v>12181.8</v>
+      </c>
+      <c r="K102">
+        <v>18800</v>
+      </c>
+      <c r="L102">
+        <v>3651.33</v>
+      </c>
+      <c r="M102">
+        <v>2856.67</v>
+      </c>
+      <c r="N102">
+        <v>4140.83</v>
+      </c>
+      <c r="O102">
+        <v>102250</v>
+      </c>
+      <c r="P102">
+        <v>145750</v>
+      </c>
+      <c r="Q102">
+        <v>5980</v>
+      </c>
+      <c r="R102">
+        <v>6100</v>
+      </c>
+      <c r="S102">
+        <v>15662.3</v>
+      </c>
+      <c r="T102">
+        <v>2522</v>
+      </c>
+      <c r="U102">
+        <v>6528.33</v>
+      </c>
+      <c r="V102">
+        <v>2616.67</v>
+      </c>
+      <c r="W102">
+        <v>1552.8</v>
+      </c>
+      <c r="X102">
+        <v>2520</v>
+      </c>
+      <c r="Y102">
+        <v>5490</v>
+      </c>
+      <c r="Z102">
+        <v>3000</v>
+      </c>
+      <c r="AA102">
+        <v>2709</v>
+      </c>
+      <c r="AB102">
+        <v>6670.91</v>
+      </c>
+      <c r="AC102">
+        <v>8371.43</v>
+      </c>
+      <c r="AD102">
+        <v>2515</v>
+      </c>
+      <c r="AE102">
+        <v>684</v>
+      </c>
+      <c r="AF102">
+        <v>5260</v>
+      </c>
+      <c r="AG102">
+        <v>6475</v>
+      </c>
+      <c r="AH102">
+        <v>9565</v>
+      </c>
+      <c r="AI102">
+        <v>3652</v>
+      </c>
+      <c r="AJ102">
+        <v>3240</v>
+      </c>
+      <c r="AK102">
+        <v>5775</v>
+      </c>
+      <c r="AL102">
+        <v>1838.93</v>
+      </c>
+      <c r="AM102">
+        <v>1976.67</v>
+      </c>
+      <c r="AN102">
+        <v>1498.33</v>
+      </c>
+      <c r="AO102">
+        <v>545.22</v>
+      </c>
+      <c r="AP102">
+        <v>3645</v>
+      </c>
+      <c r="AQ102">
+        <v>121.33</v>
+      </c>
+      <c r="AR102">
+        <v>74.67</v>
+      </c>
+      <c r="AS102">
+        <v>9054.17</v>
+      </c>
+      <c r="AT102">
+        <v>2445.45</v>
+      </c>
+    </row>
+    <row r="103" spans="1:46">
+      <c r="A103" s="1">
+        <v>101</v>
+      </c>
+      <c r="B103" t="s">
+        <v>146</v>
+      </c>
+      <c r="C103">
+        <v>51790</v>
+      </c>
+      <c r="D103">
+        <v>3957.14</v>
+      </c>
+      <c r="E103">
+        <v>25710</v>
+      </c>
+      <c r="F103">
+        <v>13930</v>
+      </c>
+      <c r="G103">
+        <v>271.98</v>
+      </c>
+      <c r="H103">
+        <v>4281.25</v>
+      </c>
+      <c r="I103">
+        <v>3980</v>
+      </c>
+      <c r="J103">
+        <v>12186.4</v>
+      </c>
+      <c r="K103">
+        <v>18650</v>
+      </c>
+      <c r="L103">
+        <v>3633.33</v>
+      </c>
+      <c r="M103">
+        <v>2856.67</v>
+      </c>
+      <c r="N103">
+        <v>4097.5</v>
+      </c>
+      <c r="O103">
+        <v>101950</v>
+      </c>
+      <c r="P103">
+        <v>145500</v>
+      </c>
+      <c r="Q103">
+        <v>5920</v>
+      </c>
+      <c r="R103">
+        <v>6100</v>
+      </c>
+      <c r="S103">
+        <v>15666.6</v>
+      </c>
+      <c r="T103">
+        <v>2522</v>
+      </c>
+      <c r="U103">
+        <v>6513.33</v>
+      </c>
+      <c r="V103">
+        <v>2616.67</v>
+      </c>
+      <c r="W103">
+        <v>1552.8</v>
+      </c>
+      <c r="X103">
+        <v>2520</v>
+      </c>
+      <c r="Y103">
+        <v>5490</v>
+      </c>
+      <c r="Z103">
+        <v>2998.33</v>
+      </c>
+      <c r="AA103">
+        <v>2704</v>
+      </c>
+      <c r="AB103">
+        <v>6610</v>
+      </c>
+      <c r="AC103">
+        <v>8371.43</v>
+      </c>
+      <c r="AD103">
+        <v>2490</v>
+      </c>
+      <c r="AE103">
+        <v>676.8</v>
+      </c>
+      <c r="AF103">
+        <v>5262.5</v>
+      </c>
+      <c r="AG103">
+        <v>6470.83</v>
+      </c>
+      <c r="AH103">
+        <v>9545</v>
+      </c>
+      <c r="AI103">
+        <v>3652</v>
+      </c>
+      <c r="AJ103">
+        <v>3232.86</v>
+      </c>
+      <c r="AK103">
+        <v>5730</v>
+      </c>
+      <c r="AL103">
+        <v>1846.43</v>
+      </c>
+      <c r="AM103">
+        <v>1976.67</v>
+      </c>
+      <c r="AN103">
+        <v>1498.33</v>
+      </c>
+      <c r="AO103">
+        <v>541.4400000000001</v>
+      </c>
+      <c r="AP103">
+        <v>3645</v>
+      </c>
+      <c r="AQ103">
+        <v>121.33</v>
+      </c>
+      <c r="AR103">
+        <v>74.67</v>
+      </c>
+      <c r="AS103">
+        <v>9054.17</v>
+      </c>
+      <c r="AT103">
+        <v>2448.18</v>
+      </c>
+    </row>
+    <row r="104" spans="1:46">
+      <c r="A104" s="1">
+        <v>102</v>
+      </c>
+      <c r="B104" t="s">
+        <v>147</v>
+      </c>
+      <c r="C104">
+        <v>51120</v>
+      </c>
+      <c r="D104">
+        <v>3891.43</v>
+      </c>
+      <c r="E104">
+        <v>25220</v>
+      </c>
+      <c r="F104">
+        <v>13990</v>
+      </c>
+      <c r="G104">
+        <v>270.68</v>
+      </c>
+      <c r="H104">
+        <v>4227.5</v>
+      </c>
+      <c r="I104">
+        <v>3980</v>
+      </c>
+      <c r="J104">
+        <v>12195.5</v>
+      </c>
+      <c r="K104">
+        <v>18600</v>
+      </c>
+      <c r="L104">
+        <v>3620</v>
+      </c>
+      <c r="M104">
+        <v>2860</v>
+      </c>
+      <c r="N104">
+        <v>4023.33</v>
+      </c>
+      <c r="O104">
+        <v>100000</v>
+      </c>
+      <c r="P104">
+        <v>146250</v>
+      </c>
+      <c r="Q104">
+        <v>5823.64</v>
+      </c>
+      <c r="R104">
+        <v>6100</v>
+      </c>
+      <c r="S104">
+        <v>15683</v>
+      </c>
+      <c r="T104">
+        <v>2522</v>
+      </c>
+      <c r="U104">
+        <v>6510</v>
+      </c>
+      <c r="V104">
+        <v>2616.67</v>
+      </c>
+      <c r="W104">
+        <v>1557.6</v>
+      </c>
+      <c r="X104">
+        <v>2520</v>
+      </c>
+      <c r="Y104">
+        <v>5515</v>
+      </c>
+      <c r="Z104">
+        <v>2998.33</v>
+      </c>
+      <c r="AA104">
+        <v>2704</v>
+      </c>
+      <c r="AB104">
+        <v>6570</v>
+      </c>
+      <c r="AC104">
+        <v>8300</v>
+      </c>
+      <c r="AD104">
+        <v>2515</v>
+      </c>
+      <c r="AE104">
+        <v>668.8</v>
+      </c>
+      <c r="AF104">
+        <v>5182.5</v>
+      </c>
+      <c r="AG104">
+        <v>6458.33</v>
+      </c>
+      <c r="AH104">
+        <v>9455</v>
+      </c>
+      <c r="AI104">
+        <v>3652</v>
+      </c>
+      <c r="AJ104">
+        <v>3224.29</v>
+      </c>
+      <c r="AK104">
+        <v>5713.75</v>
+      </c>
+      <c r="AL104">
+        <v>1852.5</v>
+      </c>
+      <c r="AM104">
+        <v>1976.67</v>
+      </c>
+      <c r="AN104">
+        <v>1498.33</v>
+      </c>
+      <c r="AO104">
+        <v>528.67</v>
+      </c>
+      <c r="AP104">
+        <v>3595</v>
+      </c>
+      <c r="AQ104">
+        <v>121.33</v>
+      </c>
+      <c r="AR104">
+        <v>74.67</v>
+      </c>
+      <c r="AS104">
+        <v>8987.5</v>
+      </c>
+      <c r="AT104">
+        <v>2454.55</v>
+      </c>
+    </row>
+    <row r="105" spans="1:46">
+      <c r="A105" s="1">
+        <v>103</v>
+      </c>
+      <c r="B105" t="s">
+        <v>148</v>
+      </c>
+      <c r="C105">
+        <v>51580</v>
+      </c>
+      <c r="D105">
+        <v>3879.29</v>
+      </c>
+      <c r="E105">
+        <v>25470</v>
+      </c>
+      <c r="F105">
+        <v>13820</v>
+      </c>
+      <c r="G105">
+        <v>270.96</v>
+      </c>
+      <c r="H105">
+        <v>4231.25</v>
+      </c>
+      <c r="I105">
+        <v>3980</v>
+      </c>
+      <c r="J105">
+        <v>12145.5</v>
+      </c>
+      <c r="K105">
+        <v>18600</v>
+      </c>
+      <c r="L105">
+        <v>3635.67</v>
+      </c>
+      <c r="M105">
+        <v>2860</v>
+      </c>
+      <c r="N105">
+        <v>4014.17</v>
+      </c>
+      <c r="O105">
+        <v>103800</v>
+      </c>
+      <c r="P105">
+        <v>146250</v>
+      </c>
+      <c r="Q105">
+        <v>5802.73</v>
+      </c>
+      <c r="R105">
+        <v>6100</v>
+      </c>
+      <c r="S105">
+        <v>15683.7</v>
+      </c>
+      <c r="T105">
+        <v>2522</v>
+      </c>
+      <c r="U105">
+        <v>6501.67</v>
+      </c>
+      <c r="V105">
+        <v>2616.67</v>
+      </c>
+      <c r="W105">
+        <v>1559.2</v>
+      </c>
+      <c r="X105">
+        <v>2513.33</v>
+      </c>
+      <c r="Y105">
+        <v>5515</v>
+      </c>
+      <c r="Z105">
+        <v>2998.33</v>
+      </c>
+      <c r="AA105">
+        <v>2704</v>
+      </c>
+      <c r="AB105">
+        <v>6510</v>
+      </c>
+      <c r="AC105">
+        <v>8278.57</v>
+      </c>
+      <c r="AD105">
+        <v>2560</v>
+      </c>
+      <c r="AE105">
+        <v>666.4</v>
+      </c>
+      <c r="AF105">
+        <v>5182.5</v>
+      </c>
+      <c r="AG105">
+        <v>6458.33</v>
+      </c>
+      <c r="AH105">
+        <v>9440</v>
+      </c>
+      <c r="AI105">
+        <v>3652</v>
+      </c>
+      <c r="AJ105">
+        <v>3150</v>
+      </c>
+      <c r="AK105">
+        <v>5705</v>
+      </c>
+      <c r="AL105">
+        <v>1852.14</v>
+      </c>
+      <c r="AM105">
+        <v>1976.67</v>
+      </c>
+      <c r="AN105">
+        <v>1498.33</v>
+      </c>
+      <c r="AO105">
+        <v>505.89</v>
+      </c>
+      <c r="AP105">
+        <v>3535</v>
+      </c>
+      <c r="AQ105">
+        <v>121.33</v>
+      </c>
+      <c r="AR105">
+        <v>74.67</v>
+      </c>
+      <c r="AS105">
+        <v>8933.33</v>
+      </c>
+      <c r="AT105">
+        <v>2459.09</v>
+      </c>
+    </row>
+    <row r="106" spans="1:46">
+      <c r="A106" s="1">
+        <v>104</v>
+      </c>
+      <c r="B106" t="s">
+        <v>149</v>
+      </c>
+      <c r="C106">
+        <v>51390</v>
+      </c>
+      <c r="D106">
+        <v>3879.29</v>
+      </c>
+      <c r="E106">
+        <v>25490</v>
+      </c>
+      <c r="F106">
+        <v>13720</v>
+      </c>
+      <c r="G106">
+        <v>270.7</v>
+      </c>
+      <c r="H106">
+        <v>4225</v>
+      </c>
+      <c r="I106">
+        <v>3980</v>
+      </c>
+      <c r="J106">
+        <v>12131.8</v>
+      </c>
+      <c r="K106">
+        <v>18350</v>
+      </c>
+      <c r="L106">
+        <v>3627</v>
+      </c>
+      <c r="M106">
+        <v>2860</v>
+      </c>
+      <c r="N106">
+        <v>4013.33</v>
+      </c>
+      <c r="O106">
+        <v>103700</v>
+      </c>
+      <c r="P106">
+        <v>146250</v>
+      </c>
+      <c r="Q106">
+        <v>5792.73</v>
+      </c>
+      <c r="R106">
+        <v>6100</v>
+      </c>
+      <c r="S106">
+        <v>15683.7</v>
+      </c>
+      <c r="T106">
+        <v>2522</v>
+      </c>
+      <c r="U106">
+        <v>6525</v>
+      </c>
+      <c r="V106">
+        <v>2616.67</v>
+      </c>
+      <c r="W106">
+        <v>1559.2</v>
+      </c>
+      <c r="X106">
+        <v>2523.33</v>
+      </c>
+      <c r="Y106">
+        <v>5515</v>
+      </c>
+      <c r="Z106">
+        <v>2998.33</v>
+      </c>
+      <c r="AA106">
+        <v>2704</v>
+      </c>
+      <c r="AB106">
+        <v>6470</v>
+      </c>
+      <c r="AC106">
+        <v>8278.57</v>
+      </c>
+      <c r="AD106">
+        <v>2620</v>
+      </c>
+      <c r="AE106">
+        <v>666.4</v>
+      </c>
+      <c r="AF106">
+        <v>5182.5</v>
+      </c>
+      <c r="AG106">
+        <v>6450</v>
+      </c>
+      <c r="AH106">
+        <v>9440</v>
+      </c>
+      <c r="AI106">
+        <v>3652</v>
+      </c>
+      <c r="AJ106">
+        <v>3170</v>
+      </c>
+      <c r="AK106">
+        <v>5723.75</v>
+      </c>
+      <c r="AL106">
+        <v>1852.5</v>
+      </c>
+      <c r="AM106">
+        <v>1976.67</v>
+      </c>
+      <c r="AN106">
+        <v>1498.33</v>
+      </c>
+      <c r="AO106">
+        <v>499.89</v>
+      </c>
+      <c r="AP106">
+        <v>3475</v>
+      </c>
+      <c r="AQ106">
+        <v>121.33</v>
+      </c>
+      <c r="AR106">
+        <v>74.67</v>
+      </c>
+      <c r="AS106">
+        <v>8887.5</v>
+      </c>
+      <c r="AT106">
+        <v>2460</v>
+      </c>
+    </row>
+    <row r="107" spans="1:46">
+      <c r="A107" s="1">
+        <v>105</v>
+      </c>
+      <c r="B107" t="s">
+        <v>150</v>
+      </c>
+      <c r="C107">
+        <v>51530</v>
+      </c>
+      <c r="D107">
+        <v>3831.43</v>
+      </c>
+      <c r="E107">
+        <v>25550</v>
+      </c>
+      <c r="F107">
+        <v>13730</v>
+      </c>
+      <c r="G107">
+        <v>271.45</v>
+      </c>
+      <c r="H107">
+        <v>4200</v>
+      </c>
+      <c r="I107">
+        <v>3963.33</v>
+      </c>
+      <c r="J107">
+        <v>12118.2</v>
+      </c>
+      <c r="K107">
+        <v>18500</v>
+      </c>
+      <c r="L107">
+        <v>3630.67</v>
+      </c>
+      <c r="M107">
+        <v>2860</v>
+      </c>
+      <c r="N107">
+        <v>3993.33</v>
+      </c>
+      <c r="O107">
+        <v>103800</v>
+      </c>
+      <c r="P107">
+        <v>145250</v>
+      </c>
+      <c r="Q107">
+        <v>5759.09</v>
+      </c>
+      <c r="R107">
+        <v>6058</v>
+      </c>
+      <c r="S107">
+        <v>15681.9</v>
+      </c>
+      <c r="T107">
+        <v>2522</v>
+      </c>
+      <c r="U107">
+        <v>6553.33</v>
+      </c>
+      <c r="V107">
+        <v>2613.33</v>
+      </c>
+      <c r="W107">
+        <v>1559.2</v>
+      </c>
+      <c r="X107">
+        <v>2523.33</v>
+      </c>
+      <c r="Y107">
+        <v>5515</v>
+      </c>
+      <c r="Z107">
+        <v>2998.33</v>
+      </c>
+      <c r="AA107">
+        <v>2700</v>
+      </c>
+      <c r="AB107">
+        <v>6435</v>
+      </c>
+      <c r="AC107">
+        <v>8192.860000000001</v>
+      </c>
+      <c r="AD107">
+        <v>2705</v>
+      </c>
+      <c r="AE107">
+        <v>664</v>
+      </c>
+      <c r="AF107">
+        <v>5182.5</v>
+      </c>
+      <c r="AG107">
+        <v>6450</v>
+      </c>
+      <c r="AH107">
+        <v>9430</v>
+      </c>
+      <c r="AI107">
+        <v>3652</v>
+      </c>
+      <c r="AJ107">
+        <v>3167.14</v>
+      </c>
+      <c r="AK107">
+        <v>5748.75</v>
+      </c>
+      <c r="AL107">
+        <v>1852.14</v>
+      </c>
+      <c r="AM107">
+        <v>1976.67</v>
+      </c>
+      <c r="AN107">
+        <v>1498.33</v>
+      </c>
+      <c r="AO107">
+        <v>497.89</v>
+      </c>
+      <c r="AP107">
+        <v>3420</v>
+      </c>
+      <c r="AQ107">
+        <v>121.67</v>
+      </c>
+      <c r="AR107">
+        <v>75</v>
+      </c>
+      <c r="AS107">
+        <v>8837.5</v>
+      </c>
+      <c r="AT107">
+        <v>2473.64</v>
+      </c>
+    </row>
+    <row r="108" spans="1:46">
+      <c r="A108" s="1">
+        <v>106</v>
+      </c>
+      <c r="B108" t="s">
+        <v>151</v>
+      </c>
+      <c r="C108">
+        <v>51870</v>
+      </c>
+      <c r="D108">
+        <v>3849.29</v>
+      </c>
+      <c r="E108">
+        <v>25160</v>
+      </c>
+      <c r="F108">
+        <v>13730</v>
+      </c>
+      <c r="G108">
+        <v>271.45</v>
+      </c>
+      <c r="H108">
+        <v>4218.75</v>
+      </c>
+      <c r="I108">
+        <v>3963.33</v>
+      </c>
+      <c r="J108">
+        <v>12118.2</v>
+      </c>
+      <c r="K108">
+        <v>18650</v>
+      </c>
+      <c r="L108">
+        <v>3630.67</v>
+      </c>
+      <c r="M108">
+        <v>2860</v>
+      </c>
+      <c r="N108">
+        <v>4016.67</v>
+      </c>
+      <c r="O108">
+        <v>103300</v>
+      </c>
+      <c r="P108">
+        <v>144750</v>
+      </c>
+      <c r="Q108">
+        <v>5765.45</v>
+      </c>
+      <c r="R108">
+        <v>6058</v>
+      </c>
+      <c r="S108">
+        <v>15674.7</v>
+      </c>
+      <c r="T108">
+        <v>2522</v>
+      </c>
+      <c r="U108">
+        <v>6521.67</v>
+      </c>
+      <c r="V108">
+        <v>2613.33</v>
+      </c>
+      <c r="W108">
+        <v>1559.2</v>
+      </c>
+      <c r="X108">
+        <v>2515</v>
+      </c>
+      <c r="Y108">
+        <v>5515</v>
+      </c>
+      <c r="Z108">
+        <v>2998.33</v>
+      </c>
+      <c r="AA108">
+        <v>2700</v>
+      </c>
+      <c r="AB108">
+        <v>6395</v>
+      </c>
+      <c r="AC108">
+        <v>8142.86</v>
+      </c>
+      <c r="AD108">
+        <v>2705</v>
+      </c>
+      <c r="AE108">
+        <v>661.6</v>
+      </c>
+      <c r="AF108">
+        <v>5182.5</v>
+      </c>
+      <c r="AG108">
+        <v>6450</v>
+      </c>
+      <c r="AH108">
+        <v>9430</v>
+      </c>
+      <c r="AI108">
+        <v>3652</v>
+      </c>
+      <c r="AJ108">
+        <v>3148.57</v>
+      </c>
+      <c r="AK108">
+        <v>5711.25</v>
+      </c>
+      <c r="AL108">
+        <v>1852.86</v>
+      </c>
+      <c r="AM108">
+        <v>1976.67</v>
+      </c>
+      <c r="AN108">
+        <v>1498.33</v>
+      </c>
+      <c r="AO108">
+        <v>502.44</v>
+      </c>
+      <c r="AP108">
+        <v>3370</v>
+      </c>
+      <c r="AQ108">
+        <v>121.67</v>
+      </c>
+      <c r="AR108">
+        <v>75</v>
+      </c>
+      <c r="AS108">
+        <v>8850</v>
+      </c>
+      <c r="AT108">
+        <v>2478.18</v>
+      </c>
+    </row>
+    <row r="109" spans="1:46">
+      <c r="A109" s="1">
+        <v>107</v>
+      </c>
+      <c r="B109" t="s">
+        <v>152</v>
+      </c>
+      <c r="C109">
+        <v>51440</v>
+      </c>
+      <c r="D109">
+        <v>3851.43</v>
+      </c>
+      <c r="E109">
+        <v>25230</v>
+      </c>
+      <c r="F109">
+        <v>13750</v>
+      </c>
+      <c r="G109">
+        <v>269.72</v>
+      </c>
+      <c r="H109">
+        <v>4222.5</v>
+      </c>
+      <c r="I109">
+        <v>3963.33</v>
+      </c>
+      <c r="J109">
+        <v>11981.8</v>
+      </c>
+      <c r="K109">
+        <v>18700</v>
+      </c>
+      <c r="L109">
+        <v>3605</v>
+      </c>
+      <c r="M109">
+        <v>2883.33</v>
+      </c>
+      <c r="N109">
+        <v>4028.33</v>
+      </c>
+      <c r="O109">
+        <v>102300</v>
+      </c>
+      <c r="P109">
+        <v>144750</v>
+      </c>
+      <c r="Q109">
+        <v>5749.09</v>
+      </c>
+      <c r="R109">
+        <v>6058</v>
+      </c>
+      <c r="S109">
+        <v>15667.6</v>
+      </c>
+      <c r="T109">
+        <v>2522</v>
+      </c>
+      <c r="U109">
+        <v>6536.67</v>
+      </c>
+      <c r="V109">
+        <v>2613.33</v>
+      </c>
+      <c r="W109">
+        <v>1559.2</v>
+      </c>
+      <c r="X109">
+        <v>2520</v>
+      </c>
+      <c r="Y109">
+        <v>5515</v>
+      </c>
+      <c r="Z109">
+        <v>2998.33</v>
+      </c>
+      <c r="AA109">
+        <v>2700</v>
+      </c>
+      <c r="AB109">
+        <v>6365</v>
+      </c>
+      <c r="AC109">
+        <v>8128.57</v>
+      </c>
+      <c r="AD109">
+        <v>2705</v>
+      </c>
+      <c r="AE109">
+        <v>660.8</v>
+      </c>
+      <c r="AF109">
+        <v>5162.5</v>
+      </c>
+      <c r="AG109">
+        <v>6445.83</v>
+      </c>
+      <c r="AH109">
+        <v>9430</v>
+      </c>
+      <c r="AI109">
+        <v>3652</v>
+      </c>
+      <c r="AJ109">
+        <v>3157.14</v>
+      </c>
+      <c r="AK109">
+        <v>5718.75</v>
+      </c>
+      <c r="AL109">
+        <v>1851.43</v>
+      </c>
+      <c r="AM109">
+        <v>1960</v>
+      </c>
+      <c r="AN109">
+        <v>1498.33</v>
+      </c>
+      <c r="AO109">
+        <v>504.44</v>
+      </c>
+      <c r="AP109">
+        <v>3370</v>
+      </c>
+      <c r="AQ109">
+        <v>121.67</v>
+      </c>
+      <c r="AR109">
+        <v>75</v>
+      </c>
+      <c r="AS109">
+        <v>8850</v>
+      </c>
+      <c r="AT109">
+        <v>2482.73</v>
+      </c>
+    </row>
+    <row r="110" spans="1:46">
+      <c r="A110" s="1">
+        <v>108</v>
+      </c>
+      <c r="B110" t="s">
+        <v>153</v>
+      </c>
+      <c r="C110">
+        <v>50910</v>
+      </c>
+      <c r="D110">
+        <v>3799.29</v>
+      </c>
+      <c r="E110">
+        <v>25260</v>
+      </c>
+      <c r="F110">
+        <v>13740</v>
+      </c>
+      <c r="G110">
+        <v>269.05</v>
+      </c>
+      <c r="H110">
+        <v>4167.5</v>
+      </c>
+      <c r="I110">
+        <v>3963.33</v>
+      </c>
+      <c r="J110">
+        <v>11909.1</v>
+      </c>
+      <c r="K110">
+        <v>18600</v>
+      </c>
+      <c r="L110">
+        <v>3587.33</v>
+      </c>
+      <c r="M110">
+        <v>2910</v>
+      </c>
+      <c r="N110">
+        <v>3995.83</v>
+      </c>
+      <c r="O110">
+        <v>101500</v>
+      </c>
+      <c r="P110">
+        <v>144750</v>
+      </c>
+      <c r="Q110">
+        <v>5754.55</v>
+      </c>
+      <c r="R110">
+        <v>6038</v>
+      </c>
+      <c r="S110">
+        <v>15650.4</v>
+      </c>
+      <c r="T110">
+        <v>2522</v>
+      </c>
+      <c r="U110">
+        <v>6540</v>
+      </c>
+      <c r="V110">
+        <v>2613.33</v>
+      </c>
+      <c r="W110">
+        <v>1559.2</v>
+      </c>
+      <c r="X110">
+        <v>2520</v>
+      </c>
+      <c r="Y110">
+        <v>5515</v>
+      </c>
+      <c r="Z110">
+        <v>2998.33</v>
+      </c>
+      <c r="AA110">
+        <v>2700</v>
+      </c>
+      <c r="AB110">
+        <v>6305</v>
+      </c>
+      <c r="AC110">
+        <v>8128.57</v>
+      </c>
+      <c r="AD110">
+        <v>2725</v>
+      </c>
+      <c r="AE110">
+        <v>660</v>
+      </c>
+      <c r="AF110">
+        <v>5162.5</v>
+      </c>
+      <c r="AG110">
+        <v>6445.83</v>
+      </c>
+      <c r="AH110">
+        <v>9430</v>
+      </c>
+      <c r="AI110">
+        <v>3652</v>
+      </c>
+      <c r="AJ110">
+        <v>3157.14</v>
+      </c>
+      <c r="AK110">
+        <v>5718.75</v>
+      </c>
+      <c r="AL110">
+        <v>1855.71</v>
+      </c>
+      <c r="AM110">
+        <v>1960</v>
+      </c>
+      <c r="AN110">
+        <v>1498.33</v>
+      </c>
+      <c r="AO110">
+        <v>501</v>
+      </c>
+      <c r="AP110">
+        <v>3295</v>
+      </c>
+      <c r="AQ110">
+        <v>121.67</v>
+      </c>
+      <c r="AR110">
+        <v>75</v>
+      </c>
+      <c r="AS110">
+        <v>8866.67</v>
+      </c>
+      <c r="AT110">
+        <v>2481.82</v>
+      </c>
+    </row>
+    <row r="111" spans="1:46">
+      <c r="A111" s="1">
+        <v>109</v>
+      </c>
+      <c r="B111" t="s">
+        <v>154</v>
+      </c>
+      <c r="C111">
+        <v>50920</v>
+      </c>
+      <c r="D111">
+        <v>3760.77</v>
+      </c>
+      <c r="E111">
+        <v>25110</v>
+      </c>
+      <c r="F111">
+        <v>13790</v>
+      </c>
+      <c r="G111">
+        <v>269.5</v>
+      </c>
+      <c r="H111">
+        <v>4148.75</v>
+      </c>
+      <c r="I111">
+        <v>3963.33</v>
+      </c>
+      <c r="J111">
+        <v>11672.7</v>
+      </c>
+      <c r="K111">
+        <v>18500</v>
+      </c>
+      <c r="L111">
+        <v>3589.33</v>
+      </c>
+      <c r="M111">
+        <v>2920</v>
+      </c>
+      <c r="N111">
+        <v>3993.33</v>
+      </c>
+      <c r="O111">
+        <v>101550</v>
+      </c>
+      <c r="P111">
+        <v>144500</v>
+      </c>
+      <c r="Q111">
+        <v>5673.64</v>
+      </c>
+      <c r="R111">
+        <v>6038</v>
+      </c>
+      <c r="S111">
+        <v>15640.9</v>
+      </c>
+      <c r="T111">
+        <v>2522</v>
+      </c>
+      <c r="U111">
+        <v>6525</v>
+      </c>
+      <c r="V111">
+        <v>2613.33</v>
+      </c>
+      <c r="W111">
+        <v>1559.2</v>
+      </c>
+      <c r="X111">
+        <v>2513.33</v>
+      </c>
+      <c r="Y111">
+        <v>5515</v>
+      </c>
+      <c r="Z111">
+        <v>2998.33</v>
+      </c>
+      <c r="AA111">
+        <v>2700</v>
+      </c>
+      <c r="AB111">
+        <v>6305</v>
+      </c>
+      <c r="AC111">
+        <v>8128.57</v>
+      </c>
+      <c r="AD111">
+        <v>2725</v>
+      </c>
+      <c r="AE111">
+        <v>659.2</v>
+      </c>
+      <c r="AF111">
+        <v>5162.5</v>
+      </c>
+      <c r="AG111">
+        <v>6445.83</v>
+      </c>
+      <c r="AH111">
+        <v>9430</v>
+      </c>
+      <c r="AI111">
+        <v>3648</v>
+      </c>
+      <c r="AJ111">
+        <v>3120</v>
+      </c>
+      <c r="AK111">
+        <v>5675</v>
+      </c>
+      <c r="AL111">
+        <v>1859.29</v>
+      </c>
+      <c r="AM111">
+        <v>1943.33</v>
+      </c>
+      <c r="AN111">
+        <v>1498.33</v>
+      </c>
+      <c r="AO111">
+        <v>485.44</v>
+      </c>
+      <c r="AP111">
+        <v>3235</v>
+      </c>
+      <c r="AQ111">
+        <v>121.67</v>
+      </c>
+      <c r="AR111">
+        <v>75</v>
+      </c>
+      <c r="AS111">
+        <v>8845.83</v>
+      </c>
+      <c r="AT111">
+        <v>2479.09</v>
+      </c>
+    </row>
+    <row r="112" spans="1:46">
+      <c r="A112" s="1">
+        <v>110</v>
+      </c>
+      <c r="B112" t="s">
+        <v>155</v>
+      </c>
+      <c r="C112">
+        <v>50540</v>
+      </c>
+      <c r="D112">
+        <v>3763.85</v>
+      </c>
+      <c r="E112">
+        <v>24900</v>
+      </c>
+      <c r="F112">
+        <v>13710</v>
+      </c>
+      <c r="G112">
+        <v>269.25</v>
+      </c>
+      <c r="H112">
+        <v>4156.25</v>
+      </c>
+      <c r="I112">
+        <v>3963.33</v>
+      </c>
+      <c r="J112">
+        <v>11581.8</v>
+      </c>
+      <c r="K112">
+        <v>18500</v>
+      </c>
+      <c r="L112">
+        <v>3581.67</v>
+      </c>
+      <c r="M112">
+        <v>2926.67</v>
+      </c>
+      <c r="N112">
+        <v>3988.33</v>
+      </c>
+      <c r="O112">
+        <v>101150</v>
+      </c>
+      <c r="P112">
+        <v>144250</v>
+      </c>
+      <c r="Q112">
+        <v>5665.45</v>
+      </c>
+      <c r="R112">
+        <v>6038</v>
+      </c>
+      <c r="S112">
+        <v>15637.3</v>
+      </c>
+      <c r="T112">
+        <v>2522</v>
+      </c>
+      <c r="U112">
+        <v>6516.67</v>
+      </c>
+      <c r="V112">
+        <v>2613.33</v>
+      </c>
+      <c r="W112">
+        <v>1559.2</v>
+      </c>
+      <c r="X112">
+        <v>2513.33</v>
+      </c>
+      <c r="Y112">
+        <v>5515</v>
+      </c>
+      <c r="Z112">
+        <v>2998.33</v>
+      </c>
+      <c r="AA112">
+        <v>2700</v>
+      </c>
+      <c r="AB112">
+        <v>6305</v>
+      </c>
+      <c r="AC112">
+        <v>8128.57</v>
+      </c>
+      <c r="AD112">
+        <v>2755</v>
+      </c>
+      <c r="AE112">
+        <v>659.2</v>
+      </c>
+      <c r="AF112">
+        <v>5117.5</v>
+      </c>
+      <c r="AG112">
+        <v>6441.67</v>
+      </c>
+      <c r="AH112">
+        <v>9430</v>
+      </c>
+      <c r="AI112">
+        <v>3648</v>
+      </c>
+      <c r="AJ112">
+        <v>3125.71</v>
+      </c>
+      <c r="AK112">
+        <v>5690</v>
+      </c>
+      <c r="AL112">
+        <v>1860.36</v>
+      </c>
+      <c r="AM112">
+        <v>1926.67</v>
+      </c>
+      <c r="AN112">
+        <v>1498.33</v>
+      </c>
+      <c r="AO112">
+        <v>479.22</v>
+      </c>
+      <c r="AP112">
+        <v>3185</v>
+      </c>
+      <c r="AQ112">
+        <v>121.67</v>
+      </c>
+      <c r="AR112">
+        <v>75</v>
+      </c>
+      <c r="AS112">
+        <v>8725</v>
+      </c>
+      <c r="AT112">
+        <v>2479.09</v>
+      </c>
+    </row>
+    <row r="113" spans="1:46">
+      <c r="A113" s="1">
+        <v>111</v>
+      </c>
+      <c r="B113" t="s">
+        <v>156</v>
+      </c>
+      <c r="C113">
+        <v>50910</v>
+      </c>
+      <c r="D113">
+        <v>3736.92</v>
+      </c>
+      <c r="E113">
+        <v>25250</v>
+      </c>
+      <c r="F113">
+        <v>13750</v>
+      </c>
+      <c r="G113">
+        <v>271.7</v>
+      </c>
+      <c r="H113">
+        <v>4138.75</v>
+      </c>
+      <c r="I113">
+        <v>3963.33</v>
+      </c>
+      <c r="J113">
+        <v>11581.8</v>
+      </c>
+      <c r="K113">
+        <v>18750</v>
+      </c>
+      <c r="L113">
+        <v>3634.33</v>
+      </c>
+      <c r="M113">
+        <v>2926.67</v>
+      </c>
+      <c r="N113">
+        <v>3978.33</v>
+      </c>
+      <c r="O113">
+        <v>101750</v>
+      </c>
+      <c r="P113">
+        <v>144500</v>
+      </c>
+      <c r="Q113">
+        <v>5672.73</v>
+      </c>
+      <c r="R113">
+        <v>6032</v>
+      </c>
+      <c r="S113">
+        <v>15636.6</v>
+      </c>
+      <c r="T113">
+        <v>2524</v>
+      </c>
+      <c r="U113">
+        <v>6508.33</v>
+      </c>
+      <c r="V113">
+        <v>2613.33</v>
+      </c>
+      <c r="W113">
+        <v>1559.2</v>
+      </c>
+      <c r="X113">
+        <v>2513.33</v>
+      </c>
+      <c r="Y113">
+        <v>5515</v>
+      </c>
+      <c r="Z113">
+        <v>2998.33</v>
+      </c>
+      <c r="AA113">
+        <v>2700</v>
+      </c>
+      <c r="AB113">
+        <v>6260</v>
+      </c>
+      <c r="AC113">
+        <v>8128.57</v>
+      </c>
+      <c r="AD113">
+        <v>2785</v>
+      </c>
+      <c r="AE113">
+        <v>657.6</v>
+      </c>
+      <c r="AF113">
+        <v>5147.5</v>
+      </c>
+      <c r="AG113">
+        <v>6441.67</v>
+      </c>
+      <c r="AH113">
+        <v>9430</v>
+      </c>
+      <c r="AI113">
+        <v>3648</v>
+      </c>
+      <c r="AJ113">
+        <v>3114.29</v>
+      </c>
+      <c r="AK113">
+        <v>5701.25</v>
+      </c>
+      <c r="AL113">
+        <v>1860.36</v>
+      </c>
+      <c r="AM113">
+        <v>1916.67</v>
+      </c>
+      <c r="AN113">
+        <v>1498.33</v>
+      </c>
+      <c r="AO113">
+        <v>478.67</v>
+      </c>
+      <c r="AP113">
+        <v>3135</v>
+      </c>
+      <c r="AQ113">
+        <v>121.67</v>
+      </c>
+      <c r="AR113">
+        <v>75</v>
+      </c>
+      <c r="AS113">
+        <v>8725</v>
+      </c>
+      <c r="AT113">
+        <v>2479.09</v>
+      </c>
+    </row>
+    <row r="114" spans="1:46">
+      <c r="A114" s="1">
+        <v>112</v>
+      </c>
+      <c r="B114" t="s">
+        <v>157</v>
+      </c>
+      <c r="C114">
+        <v>49840</v>
+      </c>
+      <c r="D114">
+        <v>3624.62</v>
+      </c>
+      <c r="E114">
+        <v>25150</v>
+      </c>
+      <c r="F114">
+        <v>13570</v>
+      </c>
+      <c r="G114">
+        <v>274.2</v>
+      </c>
+      <c r="H114">
+        <v>4013.75</v>
+      </c>
+      <c r="I114">
+        <v>3963.33</v>
+      </c>
+      <c r="J114">
+        <v>11336.4</v>
+      </c>
+      <c r="K114">
+        <v>18650</v>
+      </c>
+      <c r="L114">
+        <v>3635.33</v>
+      </c>
+      <c r="M114">
+        <v>2926.67</v>
+      </c>
+      <c r="N114">
+        <v>3881.67</v>
+      </c>
+      <c r="O114">
+        <v>98550</v>
+      </c>
+      <c r="P114">
+        <v>143500</v>
+      </c>
+      <c r="Q114">
+        <v>5620.91</v>
+      </c>
+      <c r="R114">
+        <v>6032</v>
+      </c>
+      <c r="S114">
+        <v>15630.7</v>
+      </c>
+      <c r="T114">
+        <v>2524</v>
+      </c>
+      <c r="U114">
+        <v>6505</v>
+      </c>
+      <c r="V114">
+        <v>2613.33</v>
+      </c>
+      <c r="W114">
+        <v>1563.2</v>
+      </c>
+      <c r="X114">
+        <v>2523.33</v>
+      </c>
+      <c r="Y114">
+        <v>5515</v>
+      </c>
+      <c r="Z114">
+        <v>2996.67</v>
+      </c>
+      <c r="AA114">
+        <v>2700</v>
+      </c>
+      <c r="AB114">
+        <v>6235</v>
+      </c>
+      <c r="AC114">
+        <v>8100</v>
+      </c>
+      <c r="AD114">
+        <v>2785</v>
+      </c>
+      <c r="AE114">
+        <v>654.4</v>
+      </c>
+      <c r="AF114">
+        <v>5162.5</v>
+      </c>
+      <c r="AG114">
+        <v>6441.67</v>
+      </c>
+      <c r="AH114">
+        <v>9390</v>
+      </c>
+      <c r="AI114">
+        <v>3648</v>
+      </c>
+      <c r="AJ114">
+        <v>3152.86</v>
+      </c>
+      <c r="AK114">
+        <v>5710</v>
+      </c>
+      <c r="AL114">
+        <v>1860</v>
+      </c>
+      <c r="AM114">
+        <v>1916.67</v>
+      </c>
+      <c r="AN114">
+        <v>1498.33</v>
+      </c>
+      <c r="AO114">
+        <v>478.22</v>
+      </c>
+      <c r="AP114">
+        <v>3090</v>
+      </c>
+      <c r="AQ114">
+        <v>122.33</v>
+      </c>
+      <c r="AR114">
+        <v>75.17</v>
+      </c>
+      <c r="AS114">
+        <v>8733.33</v>
+      </c>
+      <c r="AT114">
+        <v>2479.09</v>
+      </c>
+    </row>
+    <row r="115" spans="1:46">
+      <c r="A115" s="1">
+        <v>113</v>
+      </c>
+      <c r="B115" t="s">
+        <v>158</v>
+      </c>
+      <c r="C115">
+        <v>48980</v>
+      </c>
+      <c r="D115">
+        <v>3539.23</v>
+      </c>
+      <c r="E115">
+        <v>25020</v>
+      </c>
+      <c r="F115">
+        <v>13550</v>
+      </c>
+      <c r="G115">
+        <v>275.25</v>
+      </c>
+      <c r="H115">
+        <v>3953.75</v>
+      </c>
+      <c r="I115">
+        <v>3956.67</v>
+      </c>
+      <c r="J115">
+        <v>10927.3</v>
+      </c>
+      <c r="K115">
+        <v>18600</v>
+      </c>
+      <c r="L115">
+        <v>3640.67</v>
+      </c>
+      <c r="M115">
+        <v>2926.67</v>
+      </c>
+      <c r="N115">
+        <v>3829.17</v>
+      </c>
+      <c r="O115">
+        <v>97050</v>
+      </c>
+      <c r="P115">
+        <v>143000</v>
+      </c>
+      <c r="Q115">
+        <v>5603.64</v>
+      </c>
+      <c r="R115">
+        <v>6032</v>
+      </c>
+      <c r="S115">
+        <v>15620.7</v>
+      </c>
+      <c r="T115">
+        <v>2524</v>
+      </c>
+      <c r="U115">
+        <v>6511.67</v>
+      </c>
+      <c r="V115">
+        <v>2613.33</v>
+      </c>
+      <c r="W115">
+        <v>1563.2</v>
+      </c>
+      <c r="X115">
+        <v>2533.33</v>
+      </c>
+      <c r="Y115">
+        <v>5515</v>
+      </c>
+      <c r="Z115">
+        <v>2996.67</v>
+      </c>
+      <c r="AA115">
+        <v>2696</v>
+      </c>
+      <c r="AB115">
+        <v>6185</v>
+      </c>
+      <c r="AC115">
+        <v>8100</v>
+      </c>
+      <c r="AD115">
+        <v>2770</v>
+      </c>
+      <c r="AE115">
+        <v>653.4</v>
+      </c>
+      <c r="AF115">
+        <v>5162.5</v>
+      </c>
+      <c r="AG115">
+        <v>6441.67</v>
+      </c>
+      <c r="AH115">
+        <v>9400</v>
+      </c>
+      <c r="AI115">
+        <v>3648</v>
+      </c>
+      <c r="AJ115">
+        <v>3184.29</v>
+      </c>
+      <c r="AK115">
+        <v>5708.75</v>
+      </c>
+      <c r="AL115">
+        <v>1858.93</v>
+      </c>
+      <c r="AM115">
+        <v>1866.67</v>
+      </c>
+      <c r="AN115">
+        <v>1498.33</v>
+      </c>
+      <c r="AO115">
+        <v>456</v>
+      </c>
+      <c r="AP115">
+        <v>3090</v>
+      </c>
+      <c r="AQ115">
+        <v>122.67</v>
+      </c>
+      <c r="AR115">
+        <v>75</v>
+      </c>
+      <c r="AS115">
+        <v>8687.5</v>
+      </c>
+      <c r="AT115">
+        <v>2478.18</v>
+      </c>
+    </row>
+    <row r="116" spans="1:46">
+      <c r="A116" s="1">
+        <v>114</v>
+      </c>
+      <c r="B116" t="s">
+        <v>159</v>
+      </c>
+      <c r="C116">
+        <v>49310</v>
+      </c>
+      <c r="D116">
+        <v>3536.15</v>
+      </c>
+      <c r="E116">
+        <v>25380</v>
+      </c>
+      <c r="F116">
+        <v>13670</v>
+      </c>
+      <c r="G116">
+        <v>274.4</v>
+      </c>
+      <c r="H116">
+        <v>3966.25</v>
+      </c>
+      <c r="I116">
+        <v>3956.67</v>
+      </c>
+      <c r="J116">
+        <v>10845.5</v>
+      </c>
+      <c r="K116">
+        <v>18750</v>
+      </c>
+      <c r="L116">
+        <v>3642</v>
+      </c>
+      <c r="M116">
+        <v>2926.67</v>
+      </c>
+      <c r="N116">
+        <v>3832.5</v>
+      </c>
+      <c r="O116">
+        <v>97350</v>
+      </c>
+      <c r="P116">
+        <v>143000</v>
+      </c>
+      <c r="Q116">
+        <v>5583.64</v>
+      </c>
+      <c r="R116">
+        <v>6032</v>
+      </c>
+      <c r="S116">
+        <v>15609.3</v>
+      </c>
+      <c r="T116">
+        <v>2524</v>
+      </c>
+      <c r="U116">
+        <v>6483.33</v>
+      </c>
+      <c r="V116">
+        <v>2613.33</v>
+      </c>
+      <c r="W116">
+        <v>1563.2</v>
+      </c>
+      <c r="X116">
+        <v>2515</v>
+      </c>
+      <c r="Y116">
+        <v>5515</v>
+      </c>
+      <c r="Z116">
+        <v>2996.67</v>
+      </c>
+      <c r="AA116">
+        <v>2696</v>
+      </c>
+      <c r="AB116">
+        <v>6185</v>
+      </c>
+      <c r="AC116">
+        <v>8064.29</v>
+      </c>
+      <c r="AD116">
+        <v>2750</v>
+      </c>
+      <c r="AE116">
+        <v>650.4</v>
+      </c>
+      <c r="AF116">
+        <v>5162.5</v>
+      </c>
+      <c r="AG116">
+        <v>6441.67</v>
+      </c>
+      <c r="AH116">
+        <v>9400</v>
+      </c>
+      <c r="AI116">
+        <v>3648</v>
+      </c>
+      <c r="AJ116">
+        <v>3155.71</v>
+      </c>
+      <c r="AK116">
+        <v>5676.25</v>
+      </c>
+      <c r="AL116">
+        <v>1855</v>
+      </c>
+      <c r="AM116">
+        <v>1850</v>
+      </c>
+      <c r="AN116">
+        <v>1498.33</v>
+      </c>
+      <c r="AO116">
+        <v>454.67</v>
+      </c>
+      <c r="AP116">
+        <v>3145</v>
+      </c>
+      <c r="AQ116">
+        <v>122.67</v>
+      </c>
+      <c r="AR116">
+        <v>75</v>
+      </c>
+      <c r="AS116">
+        <v>8650</v>
+      </c>
+      <c r="AT116">
+        <v>2484.55</v>
+      </c>
+    </row>
+    <row r="117" spans="1:46">
+      <c r="A117" s="1">
+        <v>115</v>
+      </c>
+      <c r="B117" t="s">
+        <v>160</v>
+      </c>
+      <c r="C117">
+        <v>49210</v>
+      </c>
+      <c r="D117">
+        <v>3558.46</v>
+      </c>
+      <c r="E117">
+        <v>25380</v>
+      </c>
+      <c r="F117">
+        <v>13640</v>
+      </c>
+      <c r="G117">
+        <v>273.48</v>
+      </c>
+      <c r="H117">
+        <v>3983.75</v>
+      </c>
+      <c r="I117">
+        <v>3948.33</v>
+      </c>
+      <c r="J117">
+        <v>10827.3</v>
+      </c>
+      <c r="K117">
+        <v>18800</v>
+      </c>
+      <c r="L117">
+        <v>3624</v>
+      </c>
+      <c r="M117">
+        <v>2926.67</v>
+      </c>
+      <c r="N117">
+        <v>3833.33</v>
+      </c>
+      <c r="O117">
+        <v>97150</v>
+      </c>
+      <c r="P117">
+        <v>142500</v>
+      </c>
+      <c r="Q117">
+        <v>5537.27</v>
+      </c>
+      <c r="R117">
+        <v>6024</v>
+      </c>
+      <c r="S117">
+        <v>15573.3</v>
+      </c>
+      <c r="T117">
+        <v>2524</v>
+      </c>
+      <c r="U117">
+        <v>6463.33</v>
+      </c>
+      <c r="V117">
+        <v>2620</v>
+      </c>
+      <c r="W117">
+        <v>1564.8</v>
+      </c>
+      <c r="X117">
+        <v>2515</v>
+      </c>
+      <c r="Y117">
+        <v>5515</v>
+      </c>
+      <c r="Z117">
+        <v>2996.67</v>
+      </c>
+      <c r="AA117">
+        <v>2696</v>
+      </c>
+      <c r="AB117">
+        <v>6165</v>
+      </c>
+      <c r="AC117">
+        <v>7957.14</v>
+      </c>
+      <c r="AD117">
+        <v>2760</v>
+      </c>
+      <c r="AE117">
+        <v>638.4</v>
+      </c>
+      <c r="AF117">
+        <v>5162.5</v>
+      </c>
+      <c r="AG117">
+        <v>6441.67</v>
+      </c>
+      <c r="AH117">
+        <v>9400</v>
+      </c>
+      <c r="AI117">
+        <v>3648</v>
+      </c>
+      <c r="AJ117">
+        <v>3154.29</v>
+      </c>
+      <c r="AK117">
+        <v>5670</v>
+      </c>
+      <c r="AL117">
+        <v>1854.64</v>
+      </c>
+      <c r="AM117">
+        <v>1833.33</v>
+      </c>
+      <c r="AN117">
+        <v>1498.33</v>
+      </c>
+      <c r="AO117">
+        <v>458.11</v>
+      </c>
+      <c r="AP117">
+        <v>3200</v>
+      </c>
+      <c r="AQ117">
+        <v>122.67</v>
+      </c>
+      <c r="AR117">
+        <v>75</v>
+      </c>
+      <c r="AS117">
+        <v>8650</v>
+      </c>
+      <c r="AT117">
+        <v>2489.09</v>
+      </c>
+    </row>
+    <row r="118" spans="1:46">
+      <c r="A118" s="1">
+        <v>116</v>
+      </c>
+      <c r="B118" t="s">
+        <v>161</v>
+      </c>
+      <c r="C118">
+        <v>49530</v>
+      </c>
+      <c r="D118">
+        <v>3555.38</v>
+      </c>
+      <c r="E118">
+        <v>25210</v>
+      </c>
+      <c r="F118">
+        <v>13740</v>
+      </c>
+      <c r="G118">
+        <v>270.79</v>
+      </c>
+      <c r="H118">
+        <v>3975</v>
+      </c>
+      <c r="I118">
+        <v>3948.33</v>
+      </c>
+      <c r="J118">
+        <v>10827.3</v>
+      </c>
+      <c r="K118">
+        <v>18800</v>
+      </c>
+      <c r="L118">
+        <v>3585.33</v>
+      </c>
+      <c r="M118">
+        <v>2926.67</v>
+      </c>
+      <c r="N118">
+        <v>3835</v>
+      </c>
+      <c r="O118">
+        <v>96700</v>
+      </c>
+      <c r="P118">
+        <v>142250</v>
+      </c>
+      <c r="Q118">
+        <v>5520</v>
+      </c>
+      <c r="R118">
+        <v>6024</v>
+      </c>
+      <c r="S118">
+        <v>15560.4</v>
+      </c>
+      <c r="T118">
+        <v>2524</v>
+      </c>
+      <c r="U118">
+        <v>6460</v>
+      </c>
+      <c r="V118">
+        <v>2620</v>
+      </c>
+      <c r="W118">
+        <v>1564.8</v>
+      </c>
+      <c r="X118">
+        <v>2506.67</v>
+      </c>
+      <c r="Y118">
+        <v>5515</v>
+      </c>
+      <c r="Z118">
+        <v>2996.67</v>
+      </c>
+      <c r="AA118">
+        <v>2696</v>
+      </c>
+      <c r="AB118">
+        <v>6070</v>
+      </c>
+      <c r="AC118">
+        <v>7957.14</v>
+      </c>
+      <c r="AD118">
+        <v>2775</v>
+      </c>
+      <c r="AE118">
+        <v>638.4</v>
+      </c>
+      <c r="AF118">
+        <v>5162.5</v>
+      </c>
+      <c r="AG118">
+        <v>6379.17</v>
+      </c>
+      <c r="AH118">
+        <v>9400</v>
+      </c>
+      <c r="AI118">
+        <v>3644</v>
+      </c>
+      <c r="AJ118">
+        <v>3131.43</v>
+      </c>
+      <c r="AK118">
+        <v>5646.25</v>
+      </c>
+      <c r="AL118">
+        <v>1853.93</v>
+      </c>
+      <c r="AM118">
+        <v>1833.33</v>
+      </c>
+      <c r="AN118">
+        <v>1498.33</v>
+      </c>
+      <c r="AO118">
+        <v>454</v>
+      </c>
+      <c r="AP118">
+        <v>3220</v>
+      </c>
+      <c r="AQ118">
+        <v>122.67</v>
+      </c>
+      <c r="AR118">
+        <v>75</v>
+      </c>
+      <c r="AS118">
+        <v>8650</v>
+      </c>
+      <c r="AT118">
+        <v>2489.09</v>
+      </c>
+    </row>
+    <row r="119" spans="1:46">
+      <c r="A119" s="1">
+        <v>117</v>
+      </c>
+      <c r="B119" t="s">
+        <v>162</v>
+      </c>
+      <c r="C119">
+        <v>49780</v>
+      </c>
+      <c r="D119">
+        <v>3588.46</v>
+      </c>
+      <c r="E119">
+        <v>25190</v>
+      </c>
+      <c r="F119">
+        <v>13640</v>
+      </c>
+      <c r="G119">
+        <v>269.99</v>
+      </c>
+      <c r="H119">
+        <v>4013.75</v>
+      </c>
+      <c r="I119">
+        <v>3948.33</v>
+      </c>
+      <c r="J119">
+        <v>10654.5</v>
+      </c>
+      <c r="K119">
+        <v>18800</v>
+      </c>
+      <c r="L119">
+        <v>3589</v>
+      </c>
+      <c r="M119">
+        <v>2926.67</v>
+      </c>
+      <c r="N119">
+        <v>3838.33</v>
+      </c>
+      <c r="O119">
+        <v>98650</v>
+      </c>
+      <c r="P119">
+        <v>142750</v>
+      </c>
+      <c r="Q119">
+        <v>5550.91</v>
+      </c>
+      <c r="R119">
+        <v>6022</v>
+      </c>
+      <c r="S119">
+        <v>15532.9</v>
+      </c>
+      <c r="T119">
+        <v>2524</v>
+      </c>
+      <c r="U119">
+        <v>6460</v>
+      </c>
+      <c r="V119">
+        <v>2620</v>
+      </c>
+      <c r="W119">
+        <v>1564.8</v>
+      </c>
+      <c r="X119">
+        <v>2526.67</v>
+      </c>
+      <c r="Y119">
+        <v>5515</v>
+      </c>
+      <c r="Z119">
+        <v>2996.67</v>
+      </c>
+      <c r="AA119">
+        <v>2696</v>
+      </c>
+      <c r="AB119">
+        <v>6060</v>
+      </c>
+      <c r="AC119">
+        <v>7957.14</v>
+      </c>
+      <c r="AD119">
+        <v>2775</v>
+      </c>
+      <c r="AE119">
+        <v>638.4</v>
+      </c>
+      <c r="AF119">
+        <v>5162.5</v>
+      </c>
+      <c r="AG119">
+        <v>6316.67</v>
+      </c>
+      <c r="AH119">
+        <v>9405</v>
+      </c>
+      <c r="AI119">
+        <v>3644</v>
+      </c>
+      <c r="AJ119">
+        <v>3213.33</v>
+      </c>
+      <c r="AK119">
+        <v>5675</v>
+      </c>
+      <c r="AL119">
+        <v>1852.5</v>
+      </c>
+      <c r="AM119">
+        <v>1800</v>
+      </c>
+      <c r="AN119">
+        <v>1498.33</v>
+      </c>
+      <c r="AO119">
+        <v>453.56</v>
+      </c>
+      <c r="AP119">
+        <v>3200</v>
+      </c>
+      <c r="AQ119">
+        <v>122.67</v>
+      </c>
+      <c r="AR119">
+        <v>75</v>
+      </c>
+      <c r="AS119">
+        <v>8650</v>
+      </c>
+      <c r="AT119">
+        <v>2489.09</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>